<commit_message>
Updated for 15 seeds per controller and training condition
</commit_message>
<xml_diff>
--- a/Evaluation_Overview.xlsx
+++ b/Evaluation_Overview.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mschilling/Desktop/Submission IROS/github/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mschilling/Desktop/Submission IROS/github_new/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671A8B2C-2859-A049-B6BF-CC433B9CB415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7340" yWindow="460" windowWidth="20860" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="6120" yWindow="500" windowWidth="24360" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flat_Terrain" sheetId="1" r:id="rId1"/>
     <sheet name="Uneven_Terrain" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="43">
   <si>
     <t>TRAINED ON FLAT GROUND</t>
   </si>
@@ -114,9 +123,6 @@
     <t>TRAINED ON Heightmap 0.1</t>
   </si>
   <si>
-    <t>dppoSeed0</t>
-  </si>
-  <si>
     <t>Std.Dev.</t>
   </si>
   <si>
@@ -128,11 +134,44 @@
   <si>
     <t>dppoSeed11</t>
   </si>
+  <si>
+    <t>ppoSeed12</t>
+  </si>
+  <si>
+    <t>ppoSeed13</t>
+  </si>
+  <si>
+    <t>dppoSeed12</t>
+  </si>
+  <si>
+    <t>ppoSeed14</t>
+  </si>
+  <si>
+    <t>ppoSeed15</t>
+  </si>
+  <si>
+    <t>dppoSeed13</t>
+  </si>
+  <si>
+    <t>dppoSeed14</t>
+  </si>
+  <si>
+    <t>dppoSeed15</t>
+  </si>
+  <si>
+    <t>p-value=0.102</t>
+  </si>
+  <si>
+    <t>p-value = 0.011</t>
+  </si>
+  <si>
+    <t>using np.stats.ttest_ind_from_stats</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -217,8 +256,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -251,17 +292,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -269,6 +312,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -471,14 +517,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC1013"/>
+  <dimension ref="A1:AC1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -518,7 +564,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
@@ -849,96 +895,152 @@
       </c>
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="1"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="3">
+        <v>470.52054077100001</v>
+      </c>
+      <c r="D14" s="3">
+        <v>16.683</v>
+      </c>
+      <c r="E14" s="7">
+        <v>367.58235809299998</v>
+      </c>
+      <c r="F14" s="7">
+        <v>31.436</v>
+      </c>
+      <c r="G14" s="7">
+        <v>309.86448554999998</v>
+      </c>
+      <c r="H14" s="7">
+        <v>66.869</v>
+      </c>
+      <c r="I14" s="7">
+        <v>237.811240387</v>
+      </c>
+      <c r="J14" s="7">
+        <v>77.725999999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="7">
-        <f>AVERAGE(C3:C13)</f>
-        <v>533.73434363720003</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="C15" s="3">
+        <v>621.66256317099999</v>
+      </c>
+      <c r="D15" s="3">
+        <v>26.887</v>
+      </c>
       <c r="E15" s="7">
-        <f>AVERAGE(E3:E13)</f>
-        <v>356.83390962410004</v>
-      </c>
-      <c r="F15" s="3"/>
+        <v>617.69496765099996</v>
+      </c>
+      <c r="F15" s="7">
+        <v>28.844999999999999</v>
+      </c>
       <c r="G15" s="7">
-        <f>AVERAGE(G3:G13)</f>
-        <v>346.55592261010003</v>
-      </c>
-      <c r="H15" s="3"/>
+        <v>523.51961059600001</v>
+      </c>
+      <c r="H15" s="7">
+        <v>28.497</v>
+      </c>
       <c r="I15" s="7">
-        <f>AVERAGE(I3:I13)</f>
-        <v>287.26379933150002</v>
-      </c>
-      <c r="J15" s="3"/>
+        <v>525.50726348900002</v>
+      </c>
+      <c r="J15" s="7">
+        <v>26.030999999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="7">
-        <f>STDEVP(C4:C13)</f>
-        <v>151.65808144531709</v>
-      </c>
-      <c r="D16" s="7"/>
+      <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="3">
+        <v>629.74735961900001</v>
+      </c>
+      <c r="D16" s="3">
+        <v>16.321000000000002</v>
+      </c>
       <c r="E16" s="7">
-        <f>STDEVP(E4:E13)</f>
-        <v>90.154177303693686</v>
-      </c>
-      <c r="F16" s="7"/>
+        <v>388.40084808300003</v>
+      </c>
+      <c r="F16" s="7">
+        <v>74.384</v>
+      </c>
       <c r="G16" s="7">
-        <f>STDEVP(G4:G13)</f>
-        <v>103.5919019902728</v>
-      </c>
-      <c r="H16" s="7"/>
+        <v>284.94041101900001</v>
+      </c>
+      <c r="H16" s="7">
+        <v>110.502</v>
+      </c>
       <c r="I16" s="7">
-        <f>STDEVP(I4:I13)</f>
-        <v>105.46015869733056</v>
-      </c>
-      <c r="J16" s="7"/>
+        <v>162.937421126</v>
+      </c>
+      <c r="J16" s="7">
+        <v>88.619</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="2"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
+      <c r="A17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="3">
+        <v>630.49696350099998</v>
+      </c>
+      <c r="D17" s="3">
+        <v>14.973000000000001</v>
+      </c>
+      <c r="E17" s="7">
+        <v>217.40284513200001</v>
+      </c>
+      <c r="F17" s="7">
+        <v>128.601</v>
+      </c>
+      <c r="G17" s="7">
+        <v>128.33290867599999</v>
+      </c>
+      <c r="H17" s="7">
+        <v>111.636</v>
+      </c>
+      <c r="I17" s="7">
+        <v>67.123567206000004</v>
+      </c>
+      <c r="J17" s="7">
+        <v>67.793000000000006</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C18" s="3">
-        <v>470.52054077100001</v>
+        <v>510.73789367699999</v>
       </c>
       <c r="D18" s="3">
-        <v>16.683</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
+        <v>14.481999999999999</v>
+      </c>
+      <c r="E18" s="7">
+        <v>377.71260742200002</v>
+      </c>
+      <c r="F18" s="7">
+        <v>55.265000000000001</v>
+      </c>
+      <c r="G18" s="7">
+        <v>298.72257614099999</v>
+      </c>
+      <c r="H18" s="7">
+        <v>77.102999999999994</v>
+      </c>
+      <c r="I18" s="7">
+        <v>200.36392465099999</v>
+      </c>
+      <c r="J18" s="7">
+        <v>91.858999999999995</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="2"/>
+      <c r="A19" s="1"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="7"/>
@@ -949,443 +1051,580 @@
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="2"/>
-      <c r="C20" s="3" t="s">
+      <c r="A20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="7">
+        <f>AVERAGE(C4:C18)</f>
+        <v>546.70058380739999</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="7">
+        <f>AVERAGE(E4:E18)</f>
+        <v>369.14218150813332</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7">
+        <f>AVERAGE(G4:G18)</f>
+        <v>334.06261453886674</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7">
+        <f>AVERAGE(I4:I18)</f>
+        <v>271.09209401160007</v>
+      </c>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="7">
+        <f>STDEVP(C4:C18)</f>
+        <v>131.2294639500507</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="7">
+        <f>STDEVP(E4:E18)</f>
+        <v>105.84352841551694</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7">
+        <f>STDEVP(G4:G18)</f>
+        <v>112.94239620674948</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7">
+        <f>STDEVP(I4:I18)</f>
+        <v>125.95540270739578</v>
+      </c>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="2"/>
+      <c r="C23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3" t="s">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3" t="s">
+      <c r="F23" s="3"/>
+      <c r="G23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3" t="s">
+      <c r="H23" s="3"/>
+      <c r="I23" s="3" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="8">
-        <v>764.20923438900002</v>
-      </c>
-      <c r="D21" s="6">
-        <v>26.01348136</v>
-      </c>
-      <c r="E21" s="8">
-        <v>382.91716020000001</v>
-      </c>
-      <c r="F21" s="6">
-        <v>75.653929099999999</v>
-      </c>
-      <c r="G21" s="8">
-        <v>376.24862703299999</v>
-      </c>
-      <c r="H21" s="3">
-        <v>87.364812900000004</v>
-      </c>
-      <c r="I21" s="8">
-        <v>416.09709932300001</v>
-      </c>
-      <c r="J21" s="3">
-        <v>58.416598819999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="8">
-        <v>707.282695246</v>
-      </c>
-      <c r="D22" s="6">
-        <v>33.83622604</v>
-      </c>
-      <c r="E22" s="8">
-        <v>399.53502151499998</v>
-      </c>
-      <c r="F22" s="6">
-        <v>75.888536569999999</v>
-      </c>
-      <c r="G22" s="8">
-        <v>399.56041349100002</v>
-      </c>
-      <c r="H22" s="3">
-        <v>79.576760879999995</v>
-      </c>
-      <c r="I22" s="8">
-        <v>410.12763303700001</v>
-      </c>
-      <c r="J22" s="3">
-        <v>65.570182259999996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="8">
-        <v>570.69317703700005</v>
-      </c>
-      <c r="D23" s="6">
-        <v>39.561656429999999</v>
-      </c>
-      <c r="E23" s="8">
-        <v>432.42965297199999</v>
-      </c>
-      <c r="F23" s="6">
-        <v>71.115927659999997</v>
-      </c>
-      <c r="G23" s="8">
-        <v>378.34701108199999</v>
-      </c>
-      <c r="H23" s="3">
-        <v>110.82804950000001</v>
-      </c>
-      <c r="I23" s="8">
-        <v>315.74972365000002</v>
-      </c>
-      <c r="J23" s="3">
-        <v>119.19497130000001</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="9">
-        <v>681.35243730399998</v>
-      </c>
-      <c r="D24" s="9">
-        <f t="shared" ref="D24:D25" si="0">SQRT(C24)</f>
-        <v>26.102728541361341</v>
+        <v>17</v>
+      </c>
+      <c r="C24" s="8">
+        <v>764.20923438900002</v>
+      </c>
+      <c r="D24" s="6">
+        <v>26.01348136</v>
       </c>
       <c r="E24" s="8">
-        <v>419.875587569</v>
+        <v>382.91716020000001</v>
       </c>
       <c r="F24" s="6">
-        <v>74.188543949999996</v>
+        <v>75.653929099999999</v>
       </c>
       <c r="G24" s="8">
-        <v>436.47382705400003</v>
+        <v>376.24862703299999</v>
       </c>
       <c r="H24" s="3">
-        <v>28.32200344</v>
+        <v>87.364812900000004</v>
       </c>
       <c r="I24" s="8">
-        <v>414.30506878699998</v>
+        <v>416.09709932300001</v>
       </c>
       <c r="J24" s="3">
-        <v>47.115436459999998</v>
+        <v>58.416598819999997</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="8">
+        <v>707.282695246</v>
+      </c>
+      <c r="D25" s="6">
+        <v>33.83622604</v>
+      </c>
+      <c r="E25" s="8">
+        <v>399.53502151499998</v>
+      </c>
+      <c r="F25" s="6">
+        <v>75.888536569999999</v>
+      </c>
+      <c r="G25" s="8">
+        <v>399.56041349100002</v>
+      </c>
+      <c r="H25" s="3">
+        <v>79.576760879999995</v>
+      </c>
+      <c r="I25" s="8">
+        <v>410.12763303700001</v>
+      </c>
+      <c r="J25" s="3">
+        <v>65.570182259999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="8">
+        <v>570.69317703700005</v>
+      </c>
+      <c r="D26" s="6">
+        <v>39.561656429999999</v>
+      </c>
+      <c r="E26" s="8">
+        <v>432.42965297199999</v>
+      </c>
+      <c r="F26" s="6">
+        <v>71.115927659999997</v>
+      </c>
+      <c r="G26" s="8">
+        <v>378.34701108199999</v>
+      </c>
+      <c r="H26" s="3">
+        <v>110.82804950000001</v>
+      </c>
+      <c r="I26" s="8">
+        <v>315.74972365000002</v>
+      </c>
+      <c r="J26" s="3">
+        <v>119.19497130000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="9">
+        <v>681.35243730399998</v>
+      </c>
+      <c r="D27" s="9">
+        <f t="shared" ref="D27:D28" si="0">SQRT(C27)</f>
+        <v>26.102728541361341</v>
+      </c>
+      <c r="E27" s="8">
+        <v>419.875587569</v>
+      </c>
+      <c r="F27" s="6">
+        <v>74.188543949999996</v>
+      </c>
+      <c r="G27" s="8">
+        <v>436.47382705400003</v>
+      </c>
+      <c r="H27" s="3">
+        <v>28.32200344</v>
+      </c>
+      <c r="I27" s="8">
+        <v>414.30506878699998</v>
+      </c>
+      <c r="J27" s="3">
+        <v>47.115436459999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C28" s="9">
         <v>756.09637542200005</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D28" s="9">
         <f t="shared" si="0"/>
         <v>27.497206683988832</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E28" s="8">
         <v>377.405104526</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F28" s="6">
         <v>120.55855510000001</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G28" s="8">
         <v>367.61359919199998</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H28" s="3">
         <v>116.70101750000001</v>
       </c>
-      <c r="I25" s="8">
+      <c r="I28" s="8">
         <v>333.76228172700002</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J28" s="3">
         <v>137.91579540000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="8">
-        <v>695.85983517</v>
-      </c>
-      <c r="D26" s="6">
-        <v>24.941518330000001</v>
-      </c>
-      <c r="E26" s="8">
-        <v>145.62662810899999</v>
-      </c>
-      <c r="F26" s="6">
-        <v>141.7495423</v>
-      </c>
-      <c r="G26" s="8">
-        <v>164.49691649299999</v>
-      </c>
-      <c r="H26" s="3">
-        <v>121.1617533</v>
-      </c>
-      <c r="I26" s="8">
-        <v>99.766225108200004</v>
-      </c>
-      <c r="J26" s="3">
-        <v>86.723702320000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="8">
-        <v>733.19424548699999</v>
-      </c>
-      <c r="D27" s="6">
-        <v>56.81810918</v>
-      </c>
-      <c r="E27" s="3">
-        <v>390.3623394</v>
-      </c>
-      <c r="F27" s="3">
-        <v>143.94188260000001</v>
-      </c>
-      <c r="G27" s="8">
-        <v>419.25552349600002</v>
-      </c>
-      <c r="H27" s="3">
-        <v>110.5351574</v>
-      </c>
-      <c r="I27" s="8">
-        <v>397.56681263000002</v>
-      </c>
-      <c r="J27" s="3">
-        <v>91.529792569999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="8">
-        <v>575.66552972800002</v>
-      </c>
-      <c r="D28" s="6">
-        <v>48.78919827</v>
-      </c>
-      <c r="E28" s="3">
-        <v>378.44723929999998</v>
-      </c>
-      <c r="F28" s="3">
-        <v>87.363620130000001</v>
-      </c>
-      <c r="G28" s="8">
-        <v>358.187494211</v>
-      </c>
-      <c r="H28" s="3">
-        <v>47.631266850000003</v>
-      </c>
-      <c r="I28" s="8">
-        <v>285.52596609599999</v>
-      </c>
-      <c r="J28" s="3">
-        <v>50.656543890000002</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="3">
-        <v>598.66600000000005</v>
-      </c>
-      <c r="D29" s="3">
-        <v>30.161000000000001</v>
-      </c>
-      <c r="E29" s="3">
-        <v>364.47500000000002</v>
-      </c>
-      <c r="F29" s="3">
-        <v>113.65</v>
-      </c>
-      <c r="G29" s="3">
-        <v>385.72800000000001</v>
+        <v>22</v>
+      </c>
+      <c r="C29" s="8">
+        <v>695.85983517</v>
+      </c>
+      <c r="D29" s="6">
+        <v>24.941518330000001</v>
+      </c>
+      <c r="E29" s="8">
+        <v>145.62662810899999</v>
+      </c>
+      <c r="F29" s="6">
+        <v>141.7495423</v>
+      </c>
+      <c r="G29" s="8">
+        <v>164.49691649299999</v>
       </c>
       <c r="H29" s="3">
-        <v>118.349</v>
-      </c>
-      <c r="I29" s="3">
-        <v>375.81099999999998</v>
+        <v>121.1617533</v>
+      </c>
+      <c r="I29" s="8">
+        <v>99.766225108200004</v>
       </c>
       <c r="J29" s="3">
-        <v>125.79600000000001</v>
+        <v>86.723702320000001</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="3">
-        <v>446.23099999999999</v>
-      </c>
-      <c r="D30" s="3">
-        <v>102.80800000000001</v>
+        <v>23</v>
+      </c>
+      <c r="C30" s="8">
+        <v>733.19424548699999</v>
+      </c>
+      <c r="D30" s="6">
+        <v>56.81810918</v>
       </c>
       <c r="E30" s="3">
-        <v>420.97500000000002</v>
+        <v>390.3623394</v>
       </c>
       <c r="F30" s="3">
-        <v>52.619</v>
-      </c>
-      <c r="G30" s="3">
-        <v>428.673</v>
+        <v>143.94188260000001</v>
+      </c>
+      <c r="G30" s="8">
+        <v>419.25552349600002</v>
       </c>
       <c r="H30" s="3">
-        <v>65.682000000000002</v>
-      </c>
-      <c r="I30" s="3">
-        <v>377.91199999999998</v>
+        <v>110.5351574</v>
+      </c>
+      <c r="I30" s="8">
+        <v>397.56681263000002</v>
       </c>
       <c r="J30" s="3">
-        <v>94.001000000000005</v>
+        <v>91.529792569999998</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="1"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+      <c r="A31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="8">
+        <v>575.66552972800002</v>
+      </c>
+      <c r="D31" s="6">
+        <v>48.78919827</v>
+      </c>
+      <c r="E31" s="3">
+        <v>378.44723929999998</v>
+      </c>
+      <c r="F31" s="3">
+        <v>87.363620130000001</v>
+      </c>
+      <c r="G31" s="8">
+        <v>358.187494211</v>
+      </c>
+      <c r="H31" s="3">
+        <v>47.631266850000003</v>
+      </c>
+      <c r="I31" s="8">
+        <v>285.52596609599999</v>
+      </c>
+      <c r="J31" s="3">
+        <v>50.656543890000002</v>
+      </c>
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="7">
-        <f>AVERAGE(C21:C30)</f>
-        <v>652.92505297830007</v>
-      </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7">
-        <f>AVERAGE(E21:E30)</f>
-        <v>371.20487335910002</v>
-      </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7">
-        <f>AVERAGE(G21:G30)</f>
-        <v>371.45844120519996</v>
-      </c>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7">
-        <f>AVERAGE(I21:I30)</f>
-        <v>342.66238103581998</v>
-      </c>
-      <c r="J32" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="C32" s="3">
+        <v>598.66600000000005</v>
+      </c>
+      <c r="D32" s="3">
+        <v>30.161000000000001</v>
+      </c>
+      <c r="E32" s="3">
+        <v>364.47500000000002</v>
+      </c>
+      <c r="F32" s="3">
+        <v>113.65</v>
+      </c>
+      <c r="G32" s="3">
+        <v>385.72800000000001</v>
+      </c>
+      <c r="H32" s="3">
+        <v>118.349</v>
+      </c>
+      <c r="I32" s="3">
+        <v>375.81099999999998</v>
+      </c>
+      <c r="J32" s="3">
+        <v>125.79600000000001</v>
+      </c>
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="2" t="s">
-        <v>29</v>
+      <c r="A33" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C33" s="7">
-        <f>STDEVP(C21:C30)</f>
-        <v>96.682723776158056</v>
-      </c>
-      <c r="D33" s="7"/>
+        <v>617.38044684299996</v>
+      </c>
+      <c r="D33" s="7">
+        <v>23.706</v>
+      </c>
       <c r="E33" s="7">
-        <f>STDEVP(E21:E30)</f>
-        <v>78.053117609341328</v>
-      </c>
-      <c r="F33" s="7"/>
+        <v>433.10698302700001</v>
+      </c>
+      <c r="F33" s="7">
+        <v>54.881999999999998</v>
+      </c>
       <c r="G33" s="7">
-        <f>STDEVP(G21:G30)</f>
-        <v>73.398079127355984</v>
-      </c>
-      <c r="H33" s="7"/>
+        <v>434.88172333199998</v>
+      </c>
+      <c r="H33" s="7">
+        <v>58.194000000000003</v>
+      </c>
       <c r="I33" s="7">
-        <f>STDEVP(I21:I30)</f>
-        <v>91.377990425818012</v>
-      </c>
-      <c r="J33" s="7"/>
+        <v>381.93632817500003</v>
+      </c>
+      <c r="J33" s="7">
+        <v>90.632999999999996</v>
+      </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="2"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
+      <c r="A34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="3">
+        <v>638.92021179999995</v>
+      </c>
+      <c r="D34" s="7">
+        <v>38.65</v>
+      </c>
+      <c r="E34" s="7">
+        <v>435.51697830000001</v>
+      </c>
+      <c r="F34" s="7">
+        <v>51.219000000000001</v>
+      </c>
+      <c r="G34" s="7">
+        <v>388.92904529899999</v>
+      </c>
+      <c r="H34" s="7">
+        <v>73.971000000000004</v>
+      </c>
+      <c r="I34" s="7">
+        <v>252.09893435999999</v>
+      </c>
+      <c r="J34" s="7">
+        <v>177.01499999999999</v>
+      </c>
     </row>
     <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="3">
-        <v>638.92021179999995</v>
-      </c>
-      <c r="D35" s="7">
-        <v>38.65</v>
-      </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>721.68469360100005</v>
+      </c>
+      <c r="D35">
+        <v>37.840000000000003</v>
+      </c>
+      <c r="E35">
+        <v>402.80968740200001</v>
+      </c>
+      <c r="F35">
+        <v>102.96</v>
+      </c>
+      <c r="G35">
+        <v>421.20179412300001</v>
+      </c>
+      <c r="H35">
+        <v>113.491</v>
+      </c>
+      <c r="I35">
+        <v>440.42524530899999</v>
+      </c>
+      <c r="J35">
+        <v>41.796999999999997</v>
+      </c>
     </row>
     <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="2"/>
+      <c r="A36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36">
+        <v>551.88438090800003</v>
+      </c>
+      <c r="D36">
+        <v>58.023000000000003</v>
+      </c>
+      <c r="E36">
+        <v>434.96985472599999</v>
+      </c>
+      <c r="F36">
+        <v>47.322000000000003</v>
+      </c>
+      <c r="G36">
+        <v>421.21697757599998</v>
+      </c>
+      <c r="H36">
+        <v>55.731000000000002</v>
+      </c>
+      <c r="I36">
+        <v>301.53731915200001</v>
+      </c>
+      <c r="J36">
+        <v>124.93</v>
+      </c>
     </row>
     <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="2"/>
-    </row>
-    <row r="38" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
+      <c r="A37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37">
+        <v>640.51203551599997</v>
+      </c>
+      <c r="D37" s="3">
+        <v>30.225999999999999</v>
+      </c>
+      <c r="E37">
+        <v>411.83303569899999</v>
+      </c>
+      <c r="F37">
+        <v>71.775999999999996</v>
+      </c>
+      <c r="G37">
+        <v>411.50186988600001</v>
+      </c>
+      <c r="H37">
+        <v>70.263999999999996</v>
+      </c>
+      <c r="I37">
+        <v>342.33638627300002</v>
+      </c>
+      <c r="J37">
+        <v>122.77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="3">
+        <v>603.26277514900005</v>
+      </c>
+      <c r="D38" s="3">
+        <v>29.08</v>
+      </c>
+      <c r="E38" s="3">
+        <v>603.56788294299997</v>
+      </c>
+      <c r="F38" s="3">
+        <v>30.771999999999998</v>
+      </c>
+      <c r="G38" s="3">
+        <v>604.94907462100002</v>
+      </c>
+      <c r="H38" s="3">
+        <v>36.469000000000001</v>
+      </c>
+      <c r="I38" s="3">
+        <v>598.16535270500003</v>
+      </c>
+      <c r="J38">
+        <v>33.764000000000003</v>
+      </c>
     </row>
     <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="2"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
+      <c r="A40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="7">
+        <f>AVERAGE(C24:C38)</f>
+        <v>657.11093824000011</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="7">
+        <f>AVERAGE(E24:E38)</f>
+        <v>400.85854371253328</v>
+      </c>
+      <c r="F40" s="3"/>
+      <c r="G40" s="7">
+        <f>AVERAGE(G24:G38)</f>
+        <v>397.90612645926672</v>
+      </c>
+      <c r="H40" s="3"/>
+      <c r="I40" s="7">
+        <f>AVERAGE(I24:I38)</f>
+        <v>357.68075842214677</v>
+      </c>
+      <c r="J40" s="3"/>
     </row>
     <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="1"/>
-      <c r="C41" s="3"/>
+      <c r="A41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="7">
+        <f>STDEVP(C24:C38)</f>
+        <v>68.072177250448675</v>
+      </c>
       <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="E41" s="7">
+        <f>STDEVP(E24:E38)</f>
+        <v>87.151857749850606</v>
+      </c>
       <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
+      <c r="G41" s="7">
+        <f>STDEVP(G24:G38)</f>
+        <v>83.867543792233121</v>
+      </c>
       <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
+      <c r="I41" s="7">
+        <f>STDEVP(I24:I38)</f>
+        <v>104.92805940694883</v>
+      </c>
       <c r="J41" s="3"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1401,25 +1640,31 @@
     </row>
     <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1"/>
-      <c r="C43" s="3"/>
+      <c r="C43" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
+      <c r="G43" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
     </row>
     <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
     </row>
     <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1"/>
@@ -1445,8 +1690,8 @@
     </row>
     <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -1478,13 +1723,13 @@
     </row>
     <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="1"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
+      <c r="G50" s="9"/>
       <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
+      <c r="I50" s="9"/>
       <c r="J50" s="3"/>
     </row>
     <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1500,52 +1745,52 @@
     </row>
     <row r="52" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="1"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="7"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
     </row>
     <row r="53" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="2"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="7"/>
+      <c r="A53" s="1"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
     </row>
     <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="2"/>
+      <c r="A54" s="1"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
     </row>
     <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="1"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
+      <c r="A55" s="2"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
     </row>
     <row r="56" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="1"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
+      <c r="A56" s="2"/>
     </row>
     <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="1"/>
@@ -1602,7 +1847,7 @@
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
     </row>
-    <row r="62" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="1"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -1613,7 +1858,7 @@
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
     </row>
-    <row r="63" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="1"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -1624,7 +1869,7 @@
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
     </row>
-    <row r="64" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="1"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -1635,42 +1880,58 @@
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
     </row>
-    <row r="65" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A65" s="2"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="7"/>
-      <c r="G65" s="7"/>
-      <c r="H65" s="7"/>
-      <c r="I65" s="7"/>
-      <c r="J65" s="7"/>
-    </row>
-    <row r="66" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="1"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+    </row>
+    <row r="66" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="1"/>
-      <c r="C66" s="7"/>
-      <c r="E66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="I66" s="7"/>
-    </row>
-    <row r="67" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+    </row>
+    <row r="67" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="2"/>
+      <c r="B67" s="3"/>
       <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
       <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
       <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
       <c r="I67" s="7"/>
-    </row>
-    <row r="68" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A68" s="2"/>
-    </row>
-    <row r="69" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="J67" s="7"/>
+    </row>
+    <row r="68" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="1"/>
+      <c r="C68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="I68" s="7"/>
+    </row>
+    <row r="69" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="2"/>
-    </row>
-    <row r="70" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="C69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="G69" s="7"/>
+      <c r="I69" s="7"/>
+    </row>
+    <row r="70" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="2"/>
     </row>
     <row r="72" spans="1:10" ht="13" x14ac:dyDescent="0.15">
@@ -4499,6 +4760,20 @@
     <row r="1013" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1013" s="2"/>
     </row>
+    <row r="1014" spans="1:1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1014" s="2"/>
+    </row>
+    <row r="1015" spans="1:1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1015" s="2"/>
+    </row>
+    <row r="1016" spans="1:1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1017" spans="1:1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1018" spans="1:1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1019" spans="1:1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1020" spans="1:1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1021" spans="1:1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1022" spans="1:1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1023" spans="1:1" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4507,11 +4782,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4860,374 +5135,683 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14" s="12"/>
+      <c r="A14" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>384.38108223</v>
+      </c>
+      <c r="D14">
+        <v>65.03</v>
+      </c>
+      <c r="E14">
+        <v>337.00957153299998</v>
+      </c>
+      <c r="F14">
+        <v>55.119</v>
+      </c>
+      <c r="G14">
+        <v>371.66645965599997</v>
+      </c>
+      <c r="H14">
+        <v>53.622</v>
+      </c>
+      <c r="I14">
+        <v>399.32753692599999</v>
+      </c>
+      <c r="J14">
+        <v>22.584</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="12" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C15">
-        <v>466.5599646</v>
+        <v>396.36304930699998</v>
+      </c>
+      <c r="D15">
+        <v>68.22</v>
       </c>
       <c r="E15">
-        <v>404.94990309999997</v>
+        <v>388.47286331200002</v>
+      </c>
+      <c r="F15">
+        <v>78.787999999999997</v>
       </c>
       <c r="G15">
-        <v>388.00290059999998</v>
+        <v>390.34959724399999</v>
+      </c>
+      <c r="H15">
+        <v>70.828000000000003</v>
       </c>
       <c r="I15">
-        <v>336.93790910000001</v>
+        <v>373.43032810199998</v>
+      </c>
+      <c r="J15">
+        <v>94.748000000000005</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C16">
-        <v>39.115469840000003</v>
+        <v>401.24880493199998</v>
+      </c>
+      <c r="D16">
+        <v>13.619</v>
       </c>
       <c r="E16">
-        <v>48.657017080000003</v>
+        <v>396.51996429399998</v>
+      </c>
+      <c r="F16">
+        <v>40.667999999999999</v>
       </c>
       <c r="G16">
-        <v>59.905734320000001</v>
+        <v>380.15005001499998</v>
+      </c>
+      <c r="H16">
+        <v>57.408000000000001</v>
       </c>
       <c r="I16">
-        <v>77.181021040000005</v>
+        <v>336.53056728400003</v>
+      </c>
+      <c r="J16">
+        <v>56.456000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" s="12"/>
+      <c r="A17" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17">
+        <v>376.98747970599999</v>
+      </c>
+      <c r="D17">
+        <v>51.268999999999998</v>
+      </c>
+      <c r="E17">
+        <v>391.44089370699999</v>
+      </c>
+      <c r="F17">
+        <v>41.850999999999999</v>
+      </c>
+      <c r="G17">
+        <v>386.25042572000001</v>
+      </c>
+      <c r="H17">
+        <v>19.707000000000001</v>
+      </c>
+      <c r="I17">
+        <v>338.08613540599998</v>
+      </c>
+      <c r="J17">
+        <v>37.366</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="12" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C18">
-        <v>544.24323879999997</v>
+        <v>397.87835876499997</v>
       </c>
       <c r="D18">
-        <v>31.832603519999999</v>
+        <v>5.4320000000000004</v>
       </c>
       <c r="E18">
-        <v>427.44066409999999</v>
+        <v>365.564659882</v>
       </c>
       <c r="F18">
-        <v>71.945182549999998</v>
+        <v>36.646999999999998</v>
       </c>
       <c r="G18">
-        <v>453.83631059999999</v>
+        <v>327.88678138699998</v>
       </c>
       <c r="H18">
-        <v>47.81917035</v>
+        <v>34.453000000000003</v>
       </c>
       <c r="I18">
-        <v>429.80844930000001</v>
+        <v>274.39650455499998</v>
       </c>
       <c r="J18">
-        <v>51.080210389999998</v>
+        <v>42.06</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A19" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19">
-        <v>318.19842679999999</v>
-      </c>
-      <c r="D19">
-        <v>13.663104730000001</v>
-      </c>
-      <c r="E19">
-        <v>312.828059</v>
-      </c>
-      <c r="F19">
-        <v>16.50313955</v>
-      </c>
-      <c r="G19">
-        <v>290.9131026</v>
-      </c>
-      <c r="H19">
-        <v>28.337639500000002</v>
-      </c>
-      <c r="I19">
-        <v>244.8337507</v>
-      </c>
-      <c r="J19">
-        <v>123.902365</v>
-      </c>
+      <c r="A19" s="12"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="12" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C20">
-        <v>474.7193102</v>
-      </c>
-      <c r="D20">
-        <v>23.042719080000001</v>
+        <f>AVERAGE(C4:C18)</f>
+        <v>441.4972280893333</v>
       </c>
       <c r="E20">
-        <v>385.68860110000003</v>
-      </c>
-      <c r="F20">
-        <v>56.145977809999998</v>
+        <f>AVERAGE(E4:E18)</f>
+        <v>395.23379888853339</v>
       </c>
       <c r="G20">
-        <v>403.58025370000001</v>
-      </c>
-      <c r="H20">
-        <v>23.72057826</v>
+        <f>AVERAGE(G4:G18)</f>
+        <v>382.42215469479999</v>
       </c>
       <c r="I20">
-        <v>384.4107846</v>
-      </c>
-      <c r="J20">
-        <v>36.200323990000001</v>
+        <f>AVERAGE(I4:I18)</f>
+        <v>339.41001089153343</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="12" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C21">
-        <v>551.79995510000003</v>
-      </c>
-      <c r="D21">
-        <v>17.309213539999998</v>
+        <f>STDEVP(C4:C18)</f>
+        <v>48.003475302466036</v>
       </c>
       <c r="E21">
-        <v>394.52648959999999</v>
-      </c>
-      <c r="F21">
-        <v>49.132126229999997</v>
+        <f>STDEVP(E4:E18)</f>
+        <v>43.932637048649184</v>
       </c>
       <c r="G21">
-        <v>388.0497661</v>
-      </c>
-      <c r="H21">
-        <v>41.889453449999998</v>
+        <f>STDEVP(G4:G18)</f>
+        <v>51.232067870201469</v>
       </c>
       <c r="I21">
-        <v>249.28053779999999</v>
-      </c>
-      <c r="J21">
-        <v>58.232372359999999</v>
+        <f>STDEVP(I4:I18)</f>
+        <v>67.633573868447655</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A22" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22">
-        <v>525.83563849999996</v>
-      </c>
-      <c r="D22">
-        <v>14.54665308</v>
-      </c>
-      <c r="E22">
-        <v>445.3247298</v>
-      </c>
-      <c r="F22">
-        <v>36.536737330000001</v>
-      </c>
-      <c r="G22">
-        <v>458.23066899999998</v>
-      </c>
-      <c r="H22">
-        <v>18.438592249999999</v>
-      </c>
-      <c r="I22">
-        <v>365.58520579999998</v>
-      </c>
-      <c r="J22">
-        <v>23.59631868</v>
-      </c>
+      <c r="A22" s="12"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" s="12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C23">
-        <v>463.40567019999997</v>
+        <v>544.24323879999997</v>
       </c>
       <c r="D23">
-        <v>20.257861779999999</v>
+        <v>31.832603519999999</v>
       </c>
       <c r="E23">
-        <v>429.18583999999998</v>
+        <v>427.44066409999999</v>
       </c>
       <c r="F23">
-        <v>39.228818459999999</v>
+        <v>71.945182549999998</v>
       </c>
       <c r="G23">
-        <v>451.74190609999999</v>
+        <v>453.83631059999999</v>
       </c>
       <c r="H23">
-        <v>18.273910310000002</v>
+        <v>47.81917035</v>
       </c>
       <c r="I23">
-        <v>407.99353869999999</v>
+        <v>429.80844930000001</v>
       </c>
       <c r="J23">
-        <v>35.683014620000002</v>
+        <v>51.080210389999998</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C24">
-        <v>490.60848379999999</v>
+        <v>318.19842679999999</v>
       </c>
       <c r="D24">
-        <v>20.42170136</v>
+        <v>13.663104730000001</v>
       </c>
       <c r="E24">
-        <v>456.3805989</v>
+        <v>312.828059</v>
       </c>
       <c r="F24">
-        <v>20.022054430000001</v>
+        <v>16.50313955</v>
       </c>
       <c r="G24">
-        <v>433.11973690000002</v>
+        <v>290.9131026</v>
       </c>
       <c r="H24">
-        <v>26.604992200000002</v>
+        <v>28.337639500000002</v>
       </c>
       <c r="I24">
-        <v>379.49434059999999</v>
+        <v>244.8337507</v>
       </c>
       <c r="J24">
-        <v>33.441006479999999</v>
+        <v>123.902365</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" s="12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C25">
-        <v>435.46672569999998</v>
+        <v>474.7193102</v>
       </c>
       <c r="D25">
-        <v>25.956385709999999</v>
+        <v>23.042719080000001</v>
       </c>
       <c r="E25">
-        <v>450.54480949999999</v>
+        <v>385.68860110000003</v>
       </c>
       <c r="F25">
-        <v>28.655500450000002</v>
+        <v>56.145977809999998</v>
       </c>
       <c r="G25">
-        <v>428.7090723</v>
+        <v>403.58025370000001</v>
       </c>
       <c r="H25">
-        <v>52.894549769999998</v>
+        <v>23.72057826</v>
       </c>
       <c r="I25">
-        <v>372.96453020000001</v>
+        <v>384.4107846</v>
       </c>
       <c r="J25">
-        <v>70.438384810000002</v>
+        <v>36.200323990000001</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26" s="12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C26">
-        <v>476.2784752</v>
+        <v>551.79995510000003</v>
       </c>
       <c r="D26">
-        <v>24.913140569999999</v>
+        <v>17.309213539999998</v>
       </c>
       <c r="E26">
-        <v>455.78240640000001</v>
+        <v>394.52648959999999</v>
       </c>
       <c r="F26">
-        <v>21.623378209999998</v>
+        <v>49.132126229999997</v>
       </c>
       <c r="G26">
-        <v>446.21094490000002</v>
+        <v>388.0497661</v>
       </c>
       <c r="H26">
-        <v>19.309136129999999</v>
+        <v>41.889453449999998</v>
       </c>
       <c r="I26">
-        <v>381.6763527</v>
+        <v>249.28053779999999</v>
       </c>
       <c r="J26">
-        <v>49.333103029999997</v>
+        <v>58.232372359999999</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="12" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C27">
-        <v>380.28946300000001</v>
+        <v>525.83563849999996</v>
       </c>
       <c r="D27">
-        <v>37.934165890000003</v>
+        <v>14.54665308</v>
       </c>
       <c r="E27">
-        <v>437.78784760000002</v>
+        <v>445.3247298</v>
       </c>
       <c r="F27">
-        <v>38.673544229999997</v>
+        <v>36.536737330000001</v>
       </c>
       <c r="G27">
-        <v>440.86454300000003</v>
+        <v>458.23066899999998</v>
       </c>
       <c r="H27">
-        <v>54.119600030000001</v>
+        <v>18.438592249999999</v>
       </c>
       <c r="I27">
-        <v>413.7057921</v>
+        <v>365.58520579999998</v>
       </c>
       <c r="J27">
-        <v>49.129062650000002</v>
+        <v>23.59631868</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A28" s="12"/>
+      <c r="A28" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28">
+        <v>463.40567019999997</v>
+      </c>
+      <c r="D28">
+        <v>20.257861779999999</v>
+      </c>
+      <c r="E28">
+        <v>429.18583999999998</v>
+      </c>
+      <c r="F28">
+        <v>39.228818459999999</v>
+      </c>
+      <c r="G28">
+        <v>451.74190609999999</v>
+      </c>
+      <c r="H28">
+        <v>18.273910310000002</v>
+      </c>
+      <c r="I28">
+        <v>407.99353869999999</v>
+      </c>
+      <c r="J28">
+        <v>35.683014620000002</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A29" s="12" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C29">
-        <v>466.0845387</v>
+        <v>490.60848379999999</v>
+      </c>
+      <c r="D29">
+        <v>20.42170136</v>
       </c>
       <c r="E29">
-        <v>419.54900459999999</v>
+        <v>456.3805989</v>
+      </c>
+      <c r="F29">
+        <v>20.022054430000001</v>
       </c>
       <c r="G29">
-        <v>419.52563049999998</v>
+        <v>433.11973690000002</v>
+      </c>
+      <c r="H29">
+        <v>26.604992200000002</v>
       </c>
       <c r="I29">
-        <v>362.9753283</v>
+        <v>379.49434059999999</v>
+      </c>
+      <c r="J29">
+        <v>33.441006479999999</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30" s="12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C30">
-        <v>69.268847510000001</v>
+        <v>435.46672569999998</v>
+      </c>
+      <c r="D30">
+        <v>25.956385709999999</v>
       </c>
       <c r="E30">
-        <v>42.360794810000002</v>
+        <v>450.54480949999999</v>
+      </c>
+      <c r="F30">
+        <v>28.655500450000002</v>
       </c>
       <c r="G30">
-        <v>47.891491019999997</v>
+        <v>428.7090723</v>
+      </c>
+      <c r="H30">
+        <v>52.894549769999998</v>
       </c>
       <c r="I30">
-        <v>60.942188600000001</v>
+        <v>372.96453020000001</v>
+      </c>
+      <c r="J30">
+        <v>70.438384810000002</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A31" s="12"/>
+      <c r="A31" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>476.2784752</v>
+      </c>
+      <c r="D31">
+        <v>24.913140569999999</v>
+      </c>
+      <c r="E31">
+        <v>455.78240640000001</v>
+      </c>
+      <c r="F31">
+        <v>21.623378209999998</v>
+      </c>
+      <c r="G31">
+        <v>446.21094490000002</v>
+      </c>
+      <c r="H31">
+        <v>19.309136129999999</v>
+      </c>
+      <c r="I31">
+        <v>381.6763527</v>
+      </c>
+      <c r="J31">
+        <v>49.333103029999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A32" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32">
+        <v>380.28946300000001</v>
+      </c>
+      <c r="D32">
+        <v>37.934165890000003</v>
+      </c>
+      <c r="E32">
+        <v>437.78784760000002</v>
+      </c>
+      <c r="F32">
+        <v>38.673544229999997</v>
+      </c>
+      <c r="G32">
+        <v>440.86454300000003</v>
+      </c>
+      <c r="H32">
+        <v>54.119600030000001</v>
+      </c>
+      <c r="I32">
+        <v>413.7057921</v>
+      </c>
+      <c r="J32">
+        <v>49.129062650000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A33" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33">
+        <v>557.33223955000005</v>
+      </c>
+      <c r="D33">
+        <v>42.054000000000002</v>
+      </c>
+      <c r="E33">
+        <v>439.17726647299997</v>
+      </c>
+      <c r="F33">
+        <v>59.256999999999998</v>
+      </c>
+      <c r="G33">
+        <v>449.88273044300001</v>
+      </c>
+      <c r="H33">
+        <v>34.945</v>
+      </c>
+      <c r="I33">
+        <v>409.29831712499998</v>
+      </c>
+      <c r="J33">
+        <v>76.319999999999993</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A34" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34">
+        <v>648.81039420299999</v>
+      </c>
+      <c r="D34">
+        <v>24.021999999999998</v>
+      </c>
+      <c r="E34">
+        <v>411.51785386900002</v>
+      </c>
+      <c r="F34">
+        <v>68.772999999999996</v>
+      </c>
+      <c r="G34">
+        <v>421.82879303499999</v>
+      </c>
+      <c r="H34">
+        <v>79.572999999999993</v>
+      </c>
+      <c r="I34">
+        <v>427.40058627500002</v>
+      </c>
+      <c r="J34">
+        <v>79.317999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A35" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35">
+        <v>585.55741498199995</v>
+      </c>
+      <c r="D35">
+        <v>16.989999999999998</v>
+      </c>
+      <c r="E35">
+        <v>415.34806280999999</v>
+      </c>
+      <c r="F35">
+        <v>55.362000000000002</v>
+      </c>
+      <c r="G35">
+        <v>425.91188650300001</v>
+      </c>
+      <c r="H35">
+        <v>81.948999999999998</v>
+      </c>
+      <c r="I35">
+        <v>318.27285495500001</v>
+      </c>
+      <c r="J35">
+        <v>114.48399999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A36" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36">
+        <v>488.42492247400003</v>
+      </c>
+      <c r="D36">
+        <v>105.012</v>
+      </c>
+      <c r="E36">
+        <v>412.30359274099999</v>
+      </c>
+      <c r="F36">
+        <v>81.241</v>
+      </c>
+      <c r="G36">
+        <v>433.12448457400001</v>
+      </c>
+      <c r="H36">
+        <v>72.72</v>
+      </c>
+      <c r="I36">
+        <v>371.27879700400001</v>
+      </c>
+      <c r="J36">
+        <v>106.386</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A37" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37">
+        <v>449.40667824299999</v>
+      </c>
+      <c r="D37">
+        <v>37.161999999999999</v>
+      </c>
+      <c r="E37">
+        <v>442.06153335300002</v>
+      </c>
+      <c r="F37">
+        <v>32.569000000000003</v>
+      </c>
+      <c r="G37">
+        <v>438.450188438</v>
+      </c>
+      <c r="H37">
+        <v>96.081999999999994</v>
+      </c>
+      <c r="I37">
+        <v>410.448735005</v>
+      </c>
+      <c r="J37">
+        <v>38.286999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A38" s="12"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A39" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <f>AVERAGE(C23:C37)</f>
+        <v>492.69180245013325</v>
+      </c>
+      <c r="E39">
+        <f>AVERAGE(E23:E37)</f>
+        <v>421.05989034973334</v>
+      </c>
+      <c r="G39">
+        <f>AVERAGE(G23:G37)</f>
+        <v>424.29695921286662</v>
+      </c>
+      <c r="I39">
+        <f>AVERAGE(I23:I37)</f>
+        <v>371.09683819093334</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A40" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40">
+        <f>STDEVP(C23:C37)</f>
+        <v>79.216340156444829</v>
+      </c>
+      <c r="E40">
+        <f>STDEVP(E23:E37)</f>
+        <v>35.531069627836388</v>
+      </c>
+      <c r="G40">
+        <f>STDEVP(G23:G37)</f>
+        <v>40.087550457586104</v>
+      </c>
+      <c r="I40">
+        <f>STDEVP(I23:I37)</f>
+        <v>55.837583454291085</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A41" s="12"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A42" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>